<commit_message>
Updated scripts, removed erroneous point
</commit_message>
<xml_diff>
--- a/Publication_Data/Collars/summary_move_collars.xlsx
+++ b/Publication_Data/Collars/summary_move_collars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stlp/Desktop/Publication/Publication/Publication_Data/Collars/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stlp/Desktop/Publication/Hopland_Fire_Deer/Publication_Data/Collars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDD683-F66F-1B4D-9631-157FC5268E48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2DC00B-9927-C84F-A8D0-B612FEDB36CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="920" windowWidth="14920" windowHeight="12520" xr2:uid="{9C5DFFCB-E3A7-4765-A83C-DCE73545CFA5}"/>
+    <workbookView xWindow="900" yWindow="1420" windowWidth="14920" windowHeight="12520" xr2:uid="{9C5DFFCB-E3A7-4765-A83C-DCE73545CFA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,10 +472,14 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -535,10 +539,11 @@
         <v>50.551136360000001</v>
       </c>
       <c r="F2">
-        <v>62.979747000000003</v>
+        <v>62.692799999999998</v>
       </c>
       <c r="G2">
-        <v>1507.1389999999999</v>
+        <f>F2*24</f>
+        <v>1504.6271999999999</v>
       </c>
       <c r="H2">
         <v>0.49736936799999998</v>
@@ -553,10 +558,11 @@
         <v>46.114649679999999</v>
       </c>
       <c r="L2">
-        <v>58.64958</v>
+        <v>58.544849999999997</v>
       </c>
       <c r="M2">
-        <v>1407.59</v>
+        <f>L2*24</f>
+        <v>1405.0763999999999</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -576,10 +582,11 @@
         <v>48.537254900000001</v>
       </c>
       <c r="F3">
-        <v>84.447249999999997</v>
+        <v>84.306510000000003</v>
       </c>
       <c r="G3">
-        <v>2026.7339999999999</v>
+        <f t="shared" ref="G3:G19" si="0">F3*24</f>
+        <v>2023.3562400000001</v>
       </c>
       <c r="H3">
         <v>0.51232860999999996</v>
@@ -594,10 +601,11 @@
         <v>86.89673913</v>
       </c>
       <c r="L3">
-        <v>50.450299999999999</v>
+        <v>50.364069999999998</v>
       </c>
       <c r="M3">
-        <v>1210.807</v>
+        <f t="shared" ref="M3:M19" si="1">L3*24</f>
+        <v>1208.73768</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -617,10 +625,11 @@
         <v>61.139534879999999</v>
       </c>
       <c r="F4">
-        <v>110.3342</v>
+        <v>110.1503</v>
       </c>
       <c r="G4">
-        <v>2648.0219999999999</v>
+        <f t="shared" si="0"/>
+        <v>2643.6071999999999</v>
       </c>
       <c r="H4">
         <v>0.49997375500000002</v>
@@ -635,10 +644,11 @@
         <v>57.940528630000003</v>
       </c>
       <c r="L4">
-        <v>59.347259999999999</v>
+        <v>59.245980000000003</v>
       </c>
       <c r="M4">
-        <v>1424.3340000000001</v>
+        <f t="shared" si="1"/>
+        <v>1421.9035200000001</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -658,10 +668,11 @@
         <v>37.399305560000002</v>
       </c>
       <c r="F5">
-        <v>80.088759999999994</v>
+        <v>79.866299999999995</v>
       </c>
       <c r="G5">
-        <v>1922.13</v>
+        <f t="shared" si="0"/>
+        <v>1916.7911999999999</v>
       </c>
       <c r="H5">
         <v>0.53082990399999996</v>
@@ -676,10 +687,11 @@
         <v>40.736434109999998</v>
       </c>
       <c r="L5">
-        <v>64.969859999999997</v>
+        <v>64.57208</v>
       </c>
       <c r="M5">
-        <v>1559.277</v>
+        <f t="shared" si="1"/>
+        <v>1549.72992</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -699,10 +711,11 @@
         <v>66.793103450000004</v>
       </c>
       <c r="F6">
-        <v>79.64228</v>
+        <v>79.421049999999994</v>
       </c>
       <c r="G6">
-        <v>1911.415</v>
+        <f t="shared" si="0"/>
+        <v>1906.1052</v>
       </c>
       <c r="H6">
         <v>0.50557207100000001</v>
@@ -720,7 +733,8 @@
         <v>53.448979999999999</v>
       </c>
       <c r="M6">
-        <v>1282.7760000000001</v>
+        <f t="shared" si="1"/>
+        <v>1282.7755199999999</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -740,10 +754,11 @@
         <v>69.397959180000001</v>
       </c>
       <c r="F7">
-        <v>83.477819999999994</v>
+        <v>83.33869</v>
       </c>
       <c r="G7">
-        <v>2003.4680000000001</v>
+        <f t="shared" si="0"/>
+        <v>2000.1285600000001</v>
       </c>
       <c r="H7">
         <v>0.511954468</v>
@@ -758,10 +773,11 @@
         <v>67.828092240000004</v>
       </c>
       <c r="L7">
-        <v>67.220960000000005</v>
+        <v>67.105860000000007</v>
       </c>
       <c r="M7">
-        <v>1613.3030000000001</v>
+        <f t="shared" si="1"/>
+        <v>1610.5406400000002</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -781,10 +797,11 @@
         <v>55.028409089999997</v>
       </c>
       <c r="F8">
-        <v>87.673829999999995</v>
+        <v>87.521619999999999</v>
       </c>
       <c r="G8">
-        <v>2104.172</v>
+        <f t="shared" si="0"/>
+        <v>2100.5188800000001</v>
       </c>
       <c r="H8">
         <v>0.50786324400000005</v>
@@ -799,10 +816,11 @@
         <v>57.374741200000003</v>
       </c>
       <c r="L8">
-        <v>57.746319999999997</v>
+        <v>57.643569999999997</v>
       </c>
       <c r="M8">
-        <v>1385.912</v>
+        <f t="shared" si="1"/>
+        <v>1383.4456799999998</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -822,10 +840,11 @@
         <v>77.228329810000005</v>
       </c>
       <c r="F9">
-        <v>92.443070000000006</v>
+        <v>92.282579999999996</v>
       </c>
       <c r="G9">
-        <v>2218.634</v>
+        <f t="shared" si="0"/>
+        <v>2214.7819199999999</v>
       </c>
       <c r="H9">
         <v>0.53230914699999998</v>
@@ -840,10 +859,11 @@
         <v>66.369230770000001</v>
       </c>
       <c r="L9">
-        <v>53.47813</v>
+        <v>53.38297</v>
       </c>
       <c r="M9">
-        <v>1283.4749999999999</v>
+        <f t="shared" si="1"/>
+        <v>1281.19128</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -863,10 +883,11 @@
         <v>40.022935779999997</v>
       </c>
       <c r="F10">
-        <v>125.9808</v>
+        <v>119.7243</v>
       </c>
       <c r="G10">
-        <v>3023.5390000000002</v>
+        <f t="shared" si="0"/>
+        <v>2873.3832000000002</v>
       </c>
       <c r="H10">
         <v>0.50215596699999998</v>
@@ -881,10 +902,11 @@
         <v>48.839080459999998</v>
       </c>
       <c r="L10">
-        <v>68.136920000000003</v>
+        <v>68.015469999999993</v>
       </c>
       <c r="M10">
-        <v>1635.2860000000001</v>
+        <f t="shared" si="1"/>
+        <v>1632.3712799999998</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -904,10 +926,11 @@
         <v>53.222448980000003</v>
       </c>
       <c r="F11">
-        <v>95.54871</v>
+        <v>95.382819999999995</v>
       </c>
       <c r="G11">
-        <v>2293.1689999999999</v>
+        <f t="shared" si="0"/>
+        <v>2289.18768</v>
       </c>
       <c r="H11">
         <v>0.50075535999999998</v>
@@ -922,10 +945,11 @@
         <v>66.743589740000004</v>
       </c>
       <c r="L11">
-        <v>181.5531</v>
+        <v>181.22890000000001</v>
       </c>
       <c r="M11">
-        <v>4357.2740000000003</v>
+        <f t="shared" si="1"/>
+        <v>4349.4935999999998</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -945,10 +969,11 @@
         <v>61.136690649999998</v>
       </c>
       <c r="F12">
-        <v>88.383459999999999</v>
+        <v>88.216070000000002</v>
       </c>
       <c r="G12">
-        <v>2121.203</v>
+        <f t="shared" si="0"/>
+        <v>2117.18568</v>
       </c>
       <c r="H12">
         <v>0.50737037100000004</v>
@@ -963,10 +988,11 @@
         <v>79.185983829999998</v>
       </c>
       <c r="L12">
-        <v>52.40701</v>
+        <v>52.305050000000001</v>
       </c>
       <c r="M12">
-        <v>1257.768</v>
+        <f t="shared" si="1"/>
+        <v>1255.3212000000001</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -986,10 +1012,11 @@
         <v>64.299191370000003</v>
       </c>
       <c r="F13">
-        <v>64.820400000000006</v>
+        <v>64.697630000000004</v>
       </c>
       <c r="G13">
-        <v>1555.69</v>
+        <f t="shared" si="0"/>
+        <v>1552.7431200000001</v>
       </c>
       <c r="H13">
         <v>0.53102639699999998</v>
@@ -1004,10 +1031,11 @@
         <v>90.593314759999998</v>
       </c>
       <c r="L13">
-        <v>43.720799999999997</v>
+        <v>43.635570000000001</v>
       </c>
       <c r="M13">
-        <v>1049.299</v>
+        <f t="shared" si="1"/>
+        <v>1047.25368</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1027,10 +1055,11 @@
         <v>45.878277150000002</v>
       </c>
       <c r="F14">
-        <v>96.175759999999997</v>
+        <v>96.015469999999993</v>
       </c>
       <c r="G14">
-        <v>2308.2179999999998</v>
+        <f t="shared" si="0"/>
+        <v>2304.3712799999998</v>
       </c>
       <c r="H14">
         <v>0.51245167700000005</v>
@@ -1045,10 +1074,11 @@
         <v>49.645875250000003</v>
       </c>
       <c r="L14">
-        <v>66.982669999999999</v>
+        <v>66.867980000000003</v>
       </c>
       <c r="M14">
-        <v>1607.5840000000001</v>
+        <f t="shared" si="1"/>
+        <v>1604.8315200000002</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1072,7 +1102,8 @@
         <v>93.941299999999998</v>
       </c>
       <c r="G15">
-        <v>2254.5</v>
+        <f t="shared" si="0"/>
+        <v>2254.5911999999998</v>
       </c>
       <c r="H15">
         <v>0.4931932</v>
@@ -1087,10 +1118,11 @@
         <v>66.666667000000004</v>
       </c>
       <c r="L15">
-        <v>179.62530000000001</v>
+        <v>85.791179999999997</v>
       </c>
       <c r="M15">
-        <v>2115.5039999999999</v>
+        <f t="shared" si="1"/>
+        <v>2058.9883199999999</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1110,11 +1142,11 @@
         <v>86.2</v>
       </c>
       <c r="F16">
-        <f>113.0523/2</f>
-        <v>56.526150000000001</v>
+        <v>85.791179999999997</v>
       </c>
       <c r="G16">
-        <v>1356.627</v>
+        <f t="shared" si="0"/>
+        <v>2058.9883199999999</v>
       </c>
       <c r="H16">
         <v>0.52192110000000003</v>
@@ -1129,10 +1161,11 @@
         <v>68.083830000000006</v>
       </c>
       <c r="L16">
-        <v>162.61840000000001</v>
+        <v>79.165719999999993</v>
       </c>
       <c r="M16">
-        <v>1951.421</v>
+        <f t="shared" si="1"/>
+        <v>1899.9772799999998</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1152,10 +1185,11 @@
         <v>52.196579999999997</v>
       </c>
       <c r="F17">
-        <v>74.033289999999994</v>
+        <v>73.799009999999996</v>
       </c>
       <c r="G17">
-        <v>1776.799</v>
+        <f t="shared" si="0"/>
+        <v>1771.1762399999998</v>
       </c>
       <c r="H17">
         <v>0.4948359</v>
@@ -1170,10 +1204,11 @@
         <v>59.842590000000001</v>
       </c>
       <c r="L17">
-        <v>73.954520000000002</v>
+        <v>73.706360000000004</v>
       </c>
       <c r="M17">
-        <v>1774.9090000000001</v>
+        <f t="shared" si="1"/>
+        <v>1768.95264</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1193,10 +1228,11 @@
         <v>35.383459999999999</v>
       </c>
       <c r="F18">
-        <v>85.767219999999995</v>
+        <v>85.265659999999997</v>
       </c>
       <c r="G18">
-        <v>2058.413</v>
+        <f t="shared" si="0"/>
+        <v>2046.3758399999999</v>
       </c>
       <c r="H18">
         <v>0.5510121</v>
@@ -1211,10 +1247,11 @@
         <v>40.258330000000001</v>
       </c>
       <c r="L18">
-        <v>80.061959999999999</v>
+        <v>79.614689999999996</v>
       </c>
       <c r="M18">
-        <v>1921.4870000000001</v>
+        <f t="shared" si="1"/>
+        <v>1910.7525599999999</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1234,10 +1271,11 @@
         <v>35.265149999999998</v>
       </c>
       <c r="F19">
-        <v>58.461320000000001</v>
+        <v>58.121429999999997</v>
       </c>
       <c r="G19">
-        <v>1403.0719999999999</v>
+        <f t="shared" si="0"/>
+        <v>1394.9143199999999</v>
       </c>
       <c r="H19">
         <v>0.50466739999999999</v>
@@ -1252,10 +1290,11 @@
         <v>34.480919999999998</v>
       </c>
       <c r="L19">
-        <v>46.58258</v>
+        <v>46.320880000000002</v>
       </c>
       <c r="M19">
-        <v>1117.982</v>
+        <f t="shared" si="1"/>
+        <v>1111.7011200000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate straightness index with other movement summary
</commit_message>
<xml_diff>
--- a/Publication_Data/Collars/summary_move_collars.xlsx
+++ b/Publication_Data/Collars/summary_move_collars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stlp/Desktop/Publication/Hopland_Fire_Deer/Publication_Data/Collars/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitlyngaynor/Documents/github-repos/hopland/Hopland_Fire_Deer/Publication_Data/Collars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2DC00B-9927-C84F-A8D0-B612FEDB36CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA60417-B30F-3647-A765-7D3B98BDE137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1420" windowWidth="14920" windowHeight="12520" xr2:uid="{9C5DFFCB-E3A7-4765-A83C-DCE73545CFA5}"/>
+    <workbookView xWindow="11560" yWindow="7600" windowWidth="25600" windowHeight="15200" xr2:uid="{9C5DFFCB-E3A7-4765-A83C-DCE73545CFA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>AnimalID</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>K4</t>
+  </si>
+  <si>
+    <t>Straightness_Paired_Pre</t>
+  </si>
+  <si>
+    <t>Straightness_Paired_Post</t>
   </si>
 </sst>
 </file>
@@ -469,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552AF88D-B08D-465C-8F93-E0BF74584524}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,7 +487,7 @@
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,8 +527,14 @@
       <c r="M1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -564,8 +576,14 @@
         <f>L2*24</f>
         <v>1405.0763999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>2.4821829999999998E-3</v>
+      </c>
+      <c r="O2">
+        <v>1.205503E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -607,8 +625,14 @@
         <f t="shared" ref="M3:M19" si="1">L3*24</f>
         <v>1208.73768</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>1.7634190000000001E-2</v>
+      </c>
+      <c r="O3">
+        <v>2.527751E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -650,8 +674,14 @@
         <f t="shared" si="1"/>
         <v>1421.9035200000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>1.138217E-2</v>
+      </c>
+      <c r="O4">
+        <v>5.9585899999999997E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -693,8 +723,14 @@
         <f t="shared" si="1"/>
         <v>1549.72992</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>1.5661370000000001E-2</v>
+      </c>
+      <c r="O5">
+        <v>4.4013949999999998E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -736,8 +772,14 @@
         <f t="shared" si="1"/>
         <v>1282.7755199999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <v>1.8659889999999998E-2</v>
+      </c>
+      <c r="O6">
+        <v>1.6444529999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -779,8 +821,14 @@
         <f t="shared" si="1"/>
         <v>1610.5406400000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <v>1.051441E-2</v>
+      </c>
+      <c r="O7">
+        <v>1.1427080000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -822,8 +870,14 @@
         <f t="shared" si="1"/>
         <v>1383.4456799999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <v>3.3264470000000002E-3</v>
+      </c>
+      <c r="O8">
+        <v>1.3293340000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -865,8 +919,14 @@
         <f t="shared" si="1"/>
         <v>1281.19128</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <v>1.148972E-2</v>
+      </c>
+      <c r="O9">
+        <v>7.9209039999999994E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -908,8 +968,14 @@
         <f t="shared" si="1"/>
         <v>1632.3712799999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <v>1.5130950000000001E-2</v>
+      </c>
+      <c r="O10">
+        <v>5.6988030000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -951,8 +1017,14 @@
         <f t="shared" si="1"/>
         <v>4349.4935999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>9.0667119999999993E-3</v>
+      </c>
+      <c r="O11">
+        <v>1.4699490000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -994,8 +1066,14 @@
         <f t="shared" si="1"/>
         <v>1255.3212000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>5.9884200000000004E-3</v>
+      </c>
+      <c r="O12">
+        <v>2.223319E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1037,8 +1115,14 @@
         <f t="shared" si="1"/>
         <v>1047.25368</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <v>8.4045969999999998E-3</v>
+      </c>
+      <c r="O13">
+        <v>6.7090759999999996E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1080,8 +1164,14 @@
         <f t="shared" si="1"/>
         <v>1604.8315200000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <v>4.1845129999999999E-3</v>
+      </c>
+      <c r="O14">
+        <v>1.7935300000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1124,8 +1214,14 @@
         <f t="shared" si="1"/>
         <v>2058.9883199999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <v>6.2429829999999997E-3</v>
+      </c>
+      <c r="O15">
+        <v>3.4996270000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1167,8 +1263,14 @@
         <f t="shared" si="1"/>
         <v>1899.9772799999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <v>4.557635E-3</v>
+      </c>
+      <c r="O16">
+        <v>2.1763049999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1210,8 +1312,14 @@
         <f t="shared" si="1"/>
         <v>1768.95264</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17">
+        <v>3.2368510000000003E-2</v>
+      </c>
+      <c r="O17">
+        <v>5.6071160000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1253,8 +1361,14 @@
         <f t="shared" si="1"/>
         <v>1910.7525599999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <v>5.8244580000000002E-3</v>
+      </c>
+      <c r="O18">
+        <v>1.370646E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1295,6 +1409,12 @@
       <c r="M19">
         <f t="shared" si="1"/>
         <v>1111.7011200000002</v>
+      </c>
+      <c r="N19">
+        <v>1.6284449999999999E-2</v>
+      </c>
+      <c r="O19">
+        <v>1.0951610000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move home range size comparison into general comparison of all movement metrics (both input data & script)
</commit_message>
<xml_diff>
--- a/Publication_Data/Collars/summary_move_collars.xlsx
+++ b/Publication_Data/Collars/summary_move_collars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitlyngaynor/Documents/github-repos/hopland/Hopland_Fire_Deer/Publication_Data/Collars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA60417-B30F-3647-A765-7D3B98BDE137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A5F2DA-C137-3F46-8ECC-4CF25151350B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11560" yWindow="7600" windowWidth="25600" windowHeight="15200" xr2:uid="{9C5DFFCB-E3A7-4765-A83C-DCE73545CFA5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>AnimalID</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Straightness_Paired_Post</t>
+  </si>
+  <si>
+    <t>HR_Paired_Pre</t>
+  </si>
+  <si>
+    <t>HR_Paired_Post</t>
   </si>
 </sst>
 </file>
@@ -475,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552AF88D-B08D-465C-8F93-E0BF74584524}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,7 +493,7 @@
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +539,14 @@
       <c r="O1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -582,8 +594,14 @@
       <c r="O2">
         <v>1.205503E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <v>9.0472618000000005E-2</v>
+      </c>
+      <c r="Q2">
+        <v>0.103796438</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -631,8 +649,14 @@
       <c r="O3">
         <v>2.527751E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>0.24547934799999999</v>
+      </c>
+      <c r="Q3">
+        <v>0.214533266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -680,8 +704,14 @@
       <c r="O4">
         <v>5.9585899999999997E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <v>0.19935281899999999</v>
+      </c>
+      <c r="Q4">
+        <v>0.37893707199999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -729,8 +759,14 @@
       <c r="O5">
         <v>4.4013949999999998E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>0.13393766900000001</v>
+      </c>
+      <c r="Q5">
+        <v>0.16669730699999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -778,8 +814,14 @@
       <c r="O6">
         <v>1.6444529999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>0.127523629</v>
+      </c>
+      <c r="Q6">
+        <v>0.36674783900000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -827,8 +869,14 @@
       <c r="O7">
         <v>1.1427080000000001E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>0.20937475699999999</v>
+      </c>
+      <c r="Q7">
+        <v>0.11430267700000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -876,8 +924,14 @@
       <c r="O8">
         <v>1.3293340000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>0.12208941</v>
+      </c>
+      <c r="Q8">
+        <v>0.149890458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -925,8 +979,14 @@
       <c r="O9">
         <v>7.9209039999999994E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>0.143736906</v>
+      </c>
+      <c r="Q9">
+        <v>0.26720469099999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -974,8 +1034,14 @@
       <c r="O10">
         <v>5.6988030000000002E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <v>0.14334878600000001</v>
+      </c>
+      <c r="Q10">
+        <v>0.27474828699999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1023,8 +1089,14 @@
       <c r="O11">
         <v>1.4699490000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11">
+        <v>0.29150812300000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.322332322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1072,8 +1144,14 @@
       <c r="O12">
         <v>2.223319E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12">
+        <v>0.15678080699999999</v>
+      </c>
+      <c r="Q12">
+        <v>0.48465596599999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1121,8 +1199,14 @@
       <c r="O13">
         <v>6.7090759999999996E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <v>9.9652075000000007E-2</v>
+      </c>
+      <c r="Q13">
+        <v>0.14448039900000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1170,8 +1254,14 @@
       <c r="O14">
         <v>1.7935300000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14">
+        <v>0.15707717800000001</v>
+      </c>
+      <c r="Q14">
+        <v>0.237597541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1220,8 +1310,14 @@
       <c r="O15">
         <v>3.4996270000000003E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15">
+        <v>0.90147280399999996</v>
+      </c>
+      <c r="Q15">
+        <v>0.84183653000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1269,8 +1365,14 @@
       <c r="O16">
         <v>2.1763049999999999E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16">
+        <v>0.55318619899999999</v>
+      </c>
+      <c r="Q16">
+        <v>0.61376038499999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1318,8 +1420,14 @@
       <c r="O17">
         <v>5.6071160000000002E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17">
+        <v>0.228015143</v>
+      </c>
+      <c r="Q17">
+        <v>0.167915071</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1367,8 +1475,14 @@
       <c r="O18">
         <v>1.370646E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18">
+        <v>0.118884248</v>
+      </c>
+      <c r="Q18">
+        <v>0.16774799400000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1415,6 +1529,12 @@
       </c>
       <c r="O19">
         <v>1.0951610000000001E-2</v>
+      </c>
+      <c r="P19">
+        <v>3.1441819000000003E-2</v>
+      </c>
+      <c r="Q19">
+        <v>4.1805956999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>